<commit_message>
New architecture based on CORE2 (#20)
</commit_message>
<xml_diff>
--- a/docs/benchmarks/benchmarks_04-11.xlsx
+++ b/docs/benchmarks/benchmarks_04-11.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="41">
   <si>
     <t>MME = Maximal Matches Enumeration</t>
   </si>
@@ -79,17 +79,71 @@
     <t>RRW</t>
   </si>
   <si>
+    <t>MMDE</t>
+  </si>
+  <si>
     <t>Notice, we used linear complexity to put more weight on the centralized distribution rather than load balancing.</t>
   </si>
   <si>
     <t>MME has really bad performance due to the replicated results (CORE is really fast enumerating vs maximal matches)</t>
+  </si>
+  <si>
+    <t>tECS Distributed Enumeration</t>
+  </si>
+  <si>
+    <t>Benchmark 1</t>
+  </si>
+  <si>
+    <t>4 workers (4 JVM, 1 worker / JVM)</t>
+  </si>
+  <si>
+    <t>134 s</t>
+  </si>
+  <si>
+    <t>Distributed</t>
+  </si>
+  <si>
+    <t>Notice, how surprisingly fast is CORE2.</t>
+  </si>
+  <si>
+    <t>Achieved through benchmark1 #maximal matches =</t>
+  </si>
+  <si>
+    <t>#Matches</t>
+  </si>
+  <si>
+    <t>Verify that the #matches of core and core2 is the same</t>
+  </si>
+  <si>
+    <t>Matches</t>
+  </si>
+  <si>
+    <t>core</t>
+  </si>
+  <si>
+    <t>core2</t>
+  </si>
+  <si>
+    <t>Query1</t>
+  </si>
+  <si>
+    <t>Query2</t>
+  </si>
+  <si>
+    <t>Query3</t>
+  </si>
+  <si>
+    <t>Query4</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="7">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="d mmm yyyy"/>
+  </numFmts>
+  <fonts count="5">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -99,7 +153,6 @@
       <color theme="1"/>
       <name val="Arial"/>
     </font>
-    <font/>
     <font>
       <color rgb="FF000000"/>
       <name val="&quot;Arial&quot;"/>
@@ -109,14 +162,11 @@
       <name val="Arial"/>
     </font>
     <font>
-      <name val="Arial"/>
-    </font>
-    <font>
       <color theme="0"/>
       <name val="Arial"/>
     </font>
   </fonts>
-  <fills count="12">
+  <fills count="15">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -183,6 +233,24 @@
         <bgColor rgb="FFF3F3F3"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF9900"/>
+        <bgColor rgb="FFFF9900"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF6AA84F"/>
+        <bgColor rgb="FF6AA84F"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD9D9D9"/>
+        <bgColor rgb="FFD9D9D9"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border/>
@@ -193,20 +261,14 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="35">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -215,10 +277,10 @@
     <xf borderId="0" fillId="4" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="5" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+    <xf borderId="0" fillId="5" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="3" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -236,50 +298,74 @@
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="8" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+    <xf borderId="0" fillId="8" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment readingOrder="0" vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="9" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+    <xf borderId="0" fillId="9" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment readingOrder="0" vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="9" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="9" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="10" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+    <xf borderId="0" fillId="10" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment readingOrder="0" vertical="bottom"/>
     </xf>
-    <xf borderId="1" fillId="8" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="1" fillId="8" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="6" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="6" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="8" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="8" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="11" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="12" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="6" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="13" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="6" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="6" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="7" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="8" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="9" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="right" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="10" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="right" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="5" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="11" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="9" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="10" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" vertical="bottom"/>
+    <xf borderId="0" fillId="12" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="13" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="7" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="14" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -289,8 +375,290 @@
 </styleSheet>
 </file>
 
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart">
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr lvl="0">
+              <a:defRPr b="0">
+                <a:solidFill>
+                  <a:srgbClr val="757575"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr b="0">
+                <a:solidFill>
+                  <a:srgbClr val="757575"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+              </a:rPr>
+              <a:t>MME vs MMDE</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$42</c:f>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln cmpd="sng">
+              <a:solidFill>
+                <a:srgbClr val="4285F4"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$38:$E$38</c:f>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$42:$E$42</c:f>
+              <c:numCache/>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$43</c:f>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln cmpd="sng">
+              <a:solidFill>
+                <a:srgbClr val="EA4335"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$38:$E$38</c:f>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$43:$E$43</c:f>
+              <c:numCache/>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:axId val="1659967838"/>
+        <c:axId val="625348306"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="1659967838"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr lvl="0">
+                  <a:defRPr b="0">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                  </a:rPr>
+                  <a:t>#Maximal Matches</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:spPr/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr lvl="0">
+              <a:defRPr b="0">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="625348306"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="625348306"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="B7B7B7"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="CCCCCC">
+                  <a:alpha val="0"/>
+                </a:srgbClr>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:minorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr lvl="0">
+                  <a:defRPr b="0">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                  </a:rPr>
+                  <a:t>Time (ms)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr lvl="0">
+              <a:defRPr b="0">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1659967838"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr lvl="0">
+            <a:defRPr b="0">
+              <a:solidFill>
+                <a:srgbClr val="1A1A1A"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+            </a:defRPr>
+          </a:pPr>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+</c:chartSpace>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer">
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>561975</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="5715000" cy="3533775"/>
+    <xdr:graphicFrame>
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="1" name="Chart 1" title="Chart"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData fLocksWithSheet="0"/>
+  </xdr:oneCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -509,32 +877,32 @@
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="4"/>
-      <c r="H2" s="5"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="3"/>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="G3" s="4"/>
-      <c r="H3" s="5"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="3"/>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="G4" s="4"/>
-      <c r="H4" s="5"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="3"/>
     </row>
     <row r="5">
       <c r="A5" s="2"/>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
-      <c r="G5" s="4"/>
-      <c r="H5" s="5"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="3"/>
     </row>
     <row r="6">
-      <c r="A6" s="6" t="s">
+      <c r="A6" s="4" t="s">
         <v>4</v>
       </c>
       <c r="G6" s="2"/>
@@ -545,495 +913,934 @@
       <c r="H7" s="3"/>
     </row>
     <row r="8">
-      <c r="A8" s="7" t="s">
+      <c r="A8" s="5" t="s">
         <v>5</v>
       </c>
       <c r="G8" s="2"/>
       <c r="H8" s="3"/>
     </row>
     <row r="9">
-      <c r="A9" s="8"/>
+      <c r="A9" s="6"/>
       <c r="G9" s="2"/>
       <c r="H9" s="3"/>
-      <c r="I9" s="9" t="s">
+      <c r="I9" s="7" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="10">
       <c r="B10" s="2"/>
-      <c r="C10" s="10" t="s">
+      <c r="C10" s="8" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="11" t="s">
+      <c r="A11" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="12" t="s">
+      <c r="B11" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="F11" s="13"/>
-      <c r="G11" s="13"/>
+      <c r="F11" s="11"/>
+      <c r="G11" s="11"/>
     </row>
     <row r="12">
-      <c r="A12" s="14" t="s">
+      <c r="A12" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="B12" s="15">
+      <c r="B12" s="13">
         <v>4.0</v>
       </c>
-      <c r="C12" s="15">
+      <c r="C12" s="13">
         <v>5.0</v>
       </c>
-      <c r="D12" s="15">
+      <c r="D12" s="13">
         <v>6.0</v>
       </c>
-      <c r="E12" s="15">
+      <c r="E12" s="13">
         <v>7.0</v>
       </c>
-      <c r="F12" s="16"/>
-      <c r="G12" s="16"/>
+      <c r="F12" s="14"/>
+      <c r="G12" s="14"/>
     </row>
     <row r="13">
-      <c r="A13" s="17" t="s">
+      <c r="A13" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="B13" s="18">
+      <c r="B13" s="16">
         <v>8026.0</v>
       </c>
-      <c r="C13" s="18">
+      <c r="C13" s="16">
         <v>13423.0</v>
       </c>
-      <c r="D13" s="18">
+      <c r="D13" s="16">
         <v>28554.0</v>
       </c>
-      <c r="E13" s="18">
+      <c r="E13" s="16">
         <v>64384.0</v>
       </c>
-      <c r="F13" s="16"/>
-      <c r="G13" s="16"/>
+      <c r="F13" s="14"/>
+      <c r="G13" s="14"/>
     </row>
     <row r="14">
-      <c r="A14" s="15" t="s">
+      <c r="A14" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="B14" s="18">
+      <c r="B14" s="16">
         <v>5249.0</v>
       </c>
-      <c r="C14" s="18">
+      <c r="C14" s="16">
         <v>6163.0</v>
       </c>
-      <c r="D14" s="18">
+      <c r="D14" s="16">
         <v>7334.0</v>
       </c>
-      <c r="E14" s="18">
+      <c r="E14" s="16">
         <v>10166.0</v>
       </c>
-      <c r="F14" s="16"/>
-      <c r="G14" s="16"/>
+      <c r="F14" s="14"/>
+      <c r="G14" s="14"/>
     </row>
     <row r="15">
-      <c r="A15" s="17" t="s">
+      <c r="A15" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="B15" s="18">
+      <c r="B15" s="16">
         <v>5373.0</v>
       </c>
-      <c r="C15" s="18">
+      <c r="C15" s="16">
         <v>6462.0</v>
       </c>
-      <c r="D15" s="18">
+      <c r="D15" s="16">
         <v>8304.0</v>
       </c>
-      <c r="E15" s="18">
+      <c r="E15" s="16">
         <v>12518.0</v>
       </c>
-      <c r="F15" s="16"/>
+      <c r="F15" s="14"/>
     </row>
     <row r="16">
-      <c r="A16" s="19" t="s">
+      <c r="A16" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="B16" s="18"/>
-      <c r="C16" s="18"/>
-      <c r="D16" s="18"/>
-      <c r="E16" s="18"/>
-      <c r="F16" s="16"/>
+      <c r="B16" s="16"/>
+      <c r="C16" s="16"/>
+      <c r="D16" s="16"/>
+      <c r="E16" s="16"/>
+      <c r="F16" s="14"/>
     </row>
     <row r="17">
-      <c r="A17" s="17" t="s">
+      <c r="A17" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="B17" s="18">
+      <c r="B17" s="16">
         <v>3.873</v>
       </c>
-      <c r="C17" s="18">
+      <c r="C17" s="16">
         <v>3.873</v>
       </c>
-      <c r="D17" s="18">
+      <c r="D17" s="16">
         <v>3.87</v>
       </c>
-      <c r="E17" s="18">
+      <c r="E17" s="16">
         <v>3.872</v>
       </c>
-      <c r="F17" s="16"/>
+      <c r="F17" s="14"/>
     </row>
     <row r="18">
-      <c r="A18" s="15" t="s">
+      <c r="A18" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="B18" s="18">
+      <c r="B18" s="16">
         <v>0.079</v>
       </c>
-      <c r="C18" s="18">
+      <c r="C18" s="16">
         <v>0.03</v>
       </c>
-      <c r="D18" s="18">
+      <c r="D18" s="16">
         <v>0.012</v>
       </c>
-      <c r="E18" s="18">
+      <c r="E18" s="16">
         <v>0.005</v>
       </c>
-      <c r="F18" s="16"/>
+      <c r="F18" s="14"/>
     </row>
     <row r="19">
-      <c r="A19" s="17" t="s">
+      <c r="A19" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="B19" s="18">
+      <c r="B19" s="16">
         <v>0.272</v>
       </c>
-      <c r="C19" s="18">
+      <c r="C19" s="16">
         <v>0.039</v>
       </c>
-      <c r="D19" s="18">
+      <c r="D19" s="16">
         <v>0.015</v>
       </c>
-      <c r="E19" s="18">
+      <c r="E19" s="16">
         <v>0.007</v>
       </c>
-      <c r="F19" s="16"/>
+      <c r="F19" s="14"/>
     </row>
     <row r="20">
-      <c r="F20" s="16"/>
-      <c r="G20" s="16"/>
+      <c r="F20" s="14"/>
+      <c r="G20" s="14"/>
     </row>
     <row r="21">
-      <c r="F21" s="16"/>
-      <c r="G21" s="16"/>
+      <c r="F21" s="14"/>
+      <c r="G21" s="14"/>
     </row>
     <row r="22">
-      <c r="A22" s="8"/>
-      <c r="F22" s="16"/>
-      <c r="G22" s="16"/>
+      <c r="A22" s="6"/>
+      <c r="F22" s="14"/>
+      <c r="G22" s="14"/>
     </row>
     <row r="23">
       <c r="B23" s="2"/>
-      <c r="C23" s="10" t="s">
+      <c r="C23" s="8" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="24">
-      <c r="A24" s="20" t="s">
+      <c r="A24" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="B24" s="12" t="s">
+      <c r="B24" s="10" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="25">
-      <c r="A25" s="21" t="s">
+      <c r="A25" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="B25" s="15">
+      <c r="B25" s="13">
         <v>4.0</v>
       </c>
-      <c r="C25" s="15">
+      <c r="C25" s="13">
         <v>5.0</v>
       </c>
-      <c r="D25" s="15">
+      <c r="D25" s="13">
         <v>6.0</v>
       </c>
-      <c r="E25" s="15">
+      <c r="E25" s="13">
         <v>7.0</v>
       </c>
     </row>
     <row r="26">
-      <c r="A26" s="17" t="s">
+      <c r="A26" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="B26" s="18">
+      <c r="B26" s="16">
         <v>15052.0</v>
       </c>
-      <c r="C26" s="18">
+      <c r="C26" s="16">
         <v>37723.0</v>
       </c>
-      <c r="D26" s="18">
+      <c r="D26" s="16">
         <v>101813.0</v>
       </c>
-      <c r="E26" s="18">
+      <c r="E26" s="16">
         <v>278579.0</v>
       </c>
     </row>
     <row r="27">
-      <c r="A27" s="15" t="s">
+      <c r="A27" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="B27" s="18">
+      <c r="B27" s="16">
         <v>6254.0</v>
       </c>
-      <c r="C27" s="18">
+      <c r="C27" s="16">
         <v>8124.0</v>
       </c>
-      <c r="D27" s="18">
+      <c r="D27" s="16">
         <v>15425.0</v>
       </c>
-      <c r="E27" s="18">
+      <c r="E27" s="16">
         <v>32565.0</v>
       </c>
     </row>
     <row r="28">
-      <c r="A28" s="17" t="s">
+      <c r="A28" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="B28" s="18">
+      <c r="B28" s="16">
         <v>6262.0</v>
       </c>
-      <c r="C28" s="18">
+      <c r="C28" s="16">
         <v>9114.0</v>
       </c>
-      <c r="D28" s="18">
+      <c r="D28" s="16">
         <v>18507.0</v>
       </c>
-      <c r="E28" s="18">
+      <c r="E28" s="16">
         <v>43035.0</v>
       </c>
     </row>
     <row r="29">
-      <c r="A29" s="16"/>
-      <c r="B29" s="22"/>
-      <c r="C29" s="22"/>
-      <c r="D29" s="22"/>
-      <c r="E29" s="22"/>
+      <c r="A29" s="14"/>
+      <c r="B29" s="20"/>
+      <c r="C29" s="20"/>
+      <c r="D29" s="20"/>
+      <c r="E29" s="20"/>
     </row>
     <row r="34">
-      <c r="A34" s="7" t="s">
+      <c r="A34" s="5" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="35">
-      <c r="A35" s="23"/>
-      <c r="B35" s="24"/>
-      <c r="C35" s="24"/>
-      <c r="D35" s="24"/>
-      <c r="E35" s="24"/>
+      <c r="A35" s="14"/>
+      <c r="B35" s="20"/>
+      <c r="C35" s="20"/>
+      <c r="D35" s="20"/>
+      <c r="E35" s="20"/>
     </row>
     <row r="36">
       <c r="B36" s="2"/>
-      <c r="C36" s="10" t="s">
+      <c r="C36" s="8" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="37">
-      <c r="A37" s="25" t="s">
+      <c r="A37" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="B37" s="12" t="s">
+      <c r="B37" s="10" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="38">
-      <c r="A38" s="14" t="s">
+      <c r="A38" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="B38" s="15">
+      <c r="B38" s="13">
         <v>7.0</v>
       </c>
-      <c r="C38" s="15">
+      <c r="C38" s="13">
         <v>8.0</v>
       </c>
-      <c r="D38" s="15">
+      <c r="D38" s="13">
         <v>9.0</v>
       </c>
-      <c r="E38" s="15">
+      <c r="E38" s="13">
         <v>10.0</v>
       </c>
     </row>
     <row r="39">
-      <c r="A39" s="15" t="s">
+      <c r="A39" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="B39" s="18">
+      <c r="B39" s="16">
         <v>9427.0</v>
       </c>
-      <c r="C39" s="18">
+      <c r="C39" s="16">
         <v>16673.0</v>
       </c>
-      <c r="D39" s="18">
+      <c r="D39" s="16">
         <v>31844.0</v>
       </c>
-      <c r="E39" s="18">
+      <c r="E39" s="16">
         <v>68597.0</v>
       </c>
     </row>
     <row r="40">
-      <c r="A40" s="15" t="s">
+      <c r="A40" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="B40" s="18">
+      <c r="B40" s="16">
         <v>9436.0</v>
       </c>
-      <c r="C40" s="18">
+      <c r="C40" s="16">
         <v>15537.0</v>
       </c>
-      <c r="D40" s="18">
+      <c r="D40" s="16">
         <v>29719.0</v>
       </c>
-      <c r="E40" s="18">
+      <c r="E40" s="16">
         <v>61430.0</v>
       </c>
     </row>
     <row r="41">
-      <c r="A41" s="15" t="s">
+      <c r="A41" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="B41" s="18">
+      <c r="B41" s="16">
         <v>9411.0</v>
       </c>
-      <c r="C41" s="18">
+      <c r="C41" s="16">
         <v>15694.0</v>
       </c>
-      <c r="D41" s="18">
+      <c r="D41" s="16">
         <v>28815.0</v>
       </c>
-      <c r="E41" s="18">
+      <c r="E41" s="16">
         <v>60387.0</v>
       </c>
     </row>
     <row r="42">
-      <c r="A42" s="17" t="s">
+      <c r="A42" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="B42" s="18">
+      <c r="B42" s="16">
         <v>12345.0</v>
       </c>
-      <c r="C42" s="18">
+      <c r="C42" s="16">
         <v>22747.0</v>
       </c>
-      <c r="D42" s="18">
+      <c r="D42" s="16">
         <v>49133.0</v>
       </c>
-      <c r="E42" s="18">
+      <c r="E42" s="16">
         <v>109384.0</v>
       </c>
     </row>
     <row r="43">
-      <c r="A43" s="19" t="s">
+      <c r="A43" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="B43" s="16">
+        <v>12452.0</v>
+      </c>
+      <c r="C43" s="16">
+        <v>17510.0</v>
+      </c>
+      <c r="D43" s="16">
+        <v>42207.0</v>
+      </c>
+      <c r="E43" s="16">
+        <v>82878.0</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="B43" s="26"/>
-      <c r="C43" s="26"/>
-      <c r="D43" s="26"/>
-      <c r="E43" s="26"/>
-    </row>
-    <row r="44">
-      <c r="A44" s="27" t="s">
+      <c r="B44" s="21"/>
+      <c r="C44" s="21"/>
+      <c r="D44" s="21"/>
+      <c r="E44" s="21"/>
+    </row>
+    <row r="45">
+      <c r="A45" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="B44" s="28">
+      <c r="B45" s="16">
         <v>0.0</v>
       </c>
-      <c r="C44" s="28">
+      <c r="C45" s="16">
         <v>0.0</v>
       </c>
-      <c r="D44" s="28">
+      <c r="D45" s="16">
         <v>0.0</v>
       </c>
-      <c r="E44" s="28">
+      <c r="E45" s="16">
         <v>0.0</v>
       </c>
     </row>
-    <row r="45">
-      <c r="A45" s="15" t="s">
+    <row r="46">
+      <c r="A46" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="B45" s="18">
+      <c r="B46" s="16">
         <v>0.116</v>
       </c>
-      <c r="C45" s="18">
+      <c r="C46" s="16">
         <v>0.085</v>
       </c>
-      <c r="D45" s="18">
+      <c r="D46" s="16">
         <v>0.05</v>
       </c>
-      <c r="E45" s="18">
+      <c r="E46" s="16">
         <v>0.03</v>
       </c>
     </row>
-    <row r="46">
-      <c r="A46" s="27" t="s">
+    <row r="47">
+      <c r="A47" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="B46" s="28">
+      <c r="B47" s="16">
         <v>0.111</v>
       </c>
-      <c r="C46" s="28">
+      <c r="C47" s="16">
         <v>0.075</v>
       </c>
-      <c r="D46" s="28">
+      <c r="D47" s="16">
         <v>0.038</v>
       </c>
-      <c r="E46" s="28">
+      <c r="E47" s="16">
         <v>0.03</v>
       </c>
     </row>
-    <row r="47">
-      <c r="A47" s="17" t="s">
+    <row r="48">
+      <c r="A48" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="B47" s="18">
+      <c r="B48" s="16">
         <v>0.007</v>
       </c>
-      <c r="C47" s="18">
+      <c r="C48" s="16">
         <v>0.002</v>
       </c>
-      <c r="D47" s="18">
+      <c r="D48" s="16">
         <v>0.001</v>
       </c>
-      <c r="E47" s="18">
+      <c r="E48" s="16">
         <v>0.0</v>
       </c>
     </row>
     <row r="49">
-      <c r="A49" s="9" t="s">
+      <c r="A49" s="13" t="s">
         <v>22</v>
       </c>
+      <c r="B49" s="16">
+        <v>0.441</v>
+      </c>
+      <c r="C49" s="16">
+        <v>0.203</v>
+      </c>
+      <c r="D49" s="16">
+        <v>0.074</v>
+      </c>
+      <c r="E49" s="16">
+        <v>0.018</v>
+      </c>
     </row>
     <row r="51">
-      <c r="A51" s="9" t="s">
+      <c r="A51" s="7" t="s">
         <v>23</v>
       </c>
     </row>
+    <row r="52">
+      <c r="A52" s="7" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" s="7"/>
+      <c r="B53" s="7"/>
+      <c r="C53" s="7"/>
+      <c r="D53" s="7"/>
+      <c r="E53" s="7"/>
+      <c r="F53" s="7"/>
+      <c r="G53" s="7"/>
+    </row>
+    <row r="54">
+      <c r="A54" s="22" t="s">
+        <v>25</v>
+      </c>
+      <c r="F54" s="11"/>
+      <c r="G54" s="11"/>
+      <c r="H54" s="11"/>
+      <c r="I54" s="11"/>
+      <c r="J54" s="11"/>
+      <c r="K54" s="11"/>
+      <c r="L54" s="11"/>
+      <c r="M54" s="11"/>
+      <c r="N54" s="11"/>
+      <c r="O54" s="11"/>
+      <c r="P54" s="11"/>
+      <c r="Q54" s="11"/>
+      <c r="R54" s="11"/>
+      <c r="S54" s="11"/>
+      <c r="T54" s="11"/>
+      <c r="U54" s="11"/>
+      <c r="V54" s="11"/>
+      <c r="W54" s="11"/>
+      <c r="X54" s="11"/>
+      <c r="Y54" s="11"/>
+      <c r="Z54" s="11"/>
+    </row>
+    <row r="55">
+      <c r="A55" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="B55" s="24" t="s">
+        <v>27</v>
+      </c>
+      <c r="F55" s="11"/>
+      <c r="G55" s="11"/>
+      <c r="H55" s="11"/>
+      <c r="I55" s="11"/>
+      <c r="J55" s="11"/>
+      <c r="K55" s="11"/>
+      <c r="L55" s="11"/>
+      <c r="M55" s="11"/>
+      <c r="N55" s="11"/>
+      <c r="O55" s="11"/>
+      <c r="P55" s="11"/>
+      <c r="Q55" s="11"/>
+      <c r="R55" s="11"/>
+      <c r="S55" s="11"/>
+      <c r="T55" s="11"/>
+      <c r="U55" s="11"/>
+      <c r="V55" s="11"/>
+      <c r="W55" s="11"/>
+      <c r="X55" s="11"/>
+      <c r="Y55" s="11"/>
+      <c r="Z55" s="11"/>
+    </row>
+    <row r="56">
+      <c r="A56" s="25" t="s">
+        <v>28</v>
+      </c>
+      <c r="B56" s="26" t="s">
+        <v>9</v>
+      </c>
+      <c r="F56" s="11"/>
+      <c r="G56" s="11"/>
+      <c r="H56" s="11"/>
+      <c r="I56" s="11"/>
+      <c r="J56" s="11"/>
+      <c r="K56" s="11"/>
+      <c r="L56" s="11"/>
+      <c r="M56" s="11"/>
+      <c r="N56" s="11"/>
+      <c r="O56" s="11"/>
+      <c r="P56" s="11"/>
+      <c r="Q56" s="11"/>
+      <c r="R56" s="11"/>
+      <c r="S56" s="11"/>
+      <c r="T56" s="11"/>
+      <c r="U56" s="11"/>
+      <c r="V56" s="11"/>
+      <c r="W56" s="11"/>
+      <c r="X56" s="11"/>
+      <c r="Y56" s="11"/>
+      <c r="Z56" s="11"/>
+    </row>
+    <row r="57">
+      <c r="A57" s="27" t="s">
+        <v>10</v>
+      </c>
+      <c r="B57" s="28">
+        <v>7.0</v>
+      </c>
+      <c r="C57" s="28">
+        <v>8.0</v>
+      </c>
+      <c r="D57" s="28">
+        <v>9.0</v>
+      </c>
+      <c r="E57" s="28">
+        <v>10.0</v>
+      </c>
+      <c r="F57" s="11"/>
+      <c r="G57" s="11"/>
+      <c r="H57" s="11"/>
+      <c r="I57" s="11"/>
+      <c r="J57" s="11"/>
+      <c r="K57" s="11"/>
+      <c r="L57" s="11"/>
+      <c r="M57" s="11"/>
+      <c r="N57" s="11"/>
+      <c r="O57" s="11"/>
+      <c r="P57" s="11"/>
+      <c r="Q57" s="11"/>
+      <c r="R57" s="11"/>
+      <c r="S57" s="11"/>
+      <c r="T57" s="11"/>
+      <c r="U57" s="11"/>
+      <c r="V57" s="11"/>
+      <c r="W57" s="11"/>
+      <c r="X57" s="11"/>
+      <c r="Y57" s="11"/>
+      <c r="Z57" s="11"/>
+    </row>
+    <row r="58">
+      <c r="A58" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="B58" s="29">
+        <v>654.0</v>
+      </c>
+      <c r="C58" s="29">
+        <v>625.0</v>
+      </c>
+      <c r="D58" s="29">
+        <v>741.0</v>
+      </c>
+      <c r="E58" s="29">
+        <v>833.0</v>
+      </c>
+      <c r="F58" s="11"/>
+      <c r="G58" s="11"/>
+      <c r="H58" s="11"/>
+      <c r="I58" s="11"/>
+      <c r="J58" s="11"/>
+      <c r="K58" s="11"/>
+      <c r="L58" s="11"/>
+      <c r="M58" s="11"/>
+      <c r="N58" s="11"/>
+      <c r="O58" s="11"/>
+      <c r="P58" s="11"/>
+      <c r="Q58" s="11"/>
+      <c r="R58" s="11"/>
+      <c r="S58" s="11"/>
+      <c r="T58" s="11"/>
+      <c r="U58" s="11"/>
+      <c r="V58" s="11"/>
+      <c r="W58" s="11"/>
+      <c r="X58" s="11"/>
+      <c r="Y58" s="11"/>
+      <c r="Z58" s="11"/>
+    </row>
+    <row r="59">
+      <c r="A59" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="B59" s="29">
+        <v>770.0</v>
+      </c>
+      <c r="C59" s="29">
+        <v>760.0</v>
+      </c>
+      <c r="D59" s="29">
+        <v>633.0</v>
+      </c>
+      <c r="E59" s="29">
+        <v>770.0</v>
+      </c>
+      <c r="F59" s="11"/>
+      <c r="G59" s="11"/>
+      <c r="H59" s="11"/>
+      <c r="I59" s="11"/>
+      <c r="J59" s="11"/>
+      <c r="K59" s="11"/>
+      <c r="L59" s="11"/>
+      <c r="M59" s="11"/>
+      <c r="N59" s="11"/>
+      <c r="O59" s="11"/>
+      <c r="P59" s="11"/>
+      <c r="Q59" s="11"/>
+      <c r="R59" s="11"/>
+      <c r="S59" s="11"/>
+      <c r="T59" s="11"/>
+      <c r="U59" s="11"/>
+      <c r="V59" s="11"/>
+      <c r="W59" s="11"/>
+      <c r="X59" s="11"/>
+      <c r="Y59" s="11"/>
+      <c r="Z59" s="11"/>
+    </row>
+    <row r="60">
+      <c r="A60" s="7"/>
+      <c r="B60" s="7"/>
+      <c r="C60" s="7"/>
+      <c r="D60" s="7"/>
+      <c r="E60" s="7"/>
+      <c r="F60" s="7"/>
+      <c r="G60" s="7"/>
+    </row>
+    <row r="61">
+      <c r="A61" s="7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" s="30">
+        <v>44551.0</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" s="31" t="s">
+        <v>25</v>
+      </c>
+      <c r="F64" s="7" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" s="32" t="s">
+        <v>26</v>
+      </c>
+      <c r="B65" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="F65" s="7">
+        <v>13.0</v>
+      </c>
+      <c r="G65" s="7">
+        <v>16.0</v>
+      </c>
+      <c r="H65" s="7">
+        <v>20.0</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" s="9"/>
+      <c r="B66" s="10" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="B67" s="13">
+        <v>769.0</v>
+      </c>
+      <c r="C67" s="13">
+        <v>1793.0</v>
+      </c>
+      <c r="D67" s="13">
+        <v>4097.0</v>
+      </c>
+      <c r="E67" s="13">
+        <v>9217.0</v>
+      </c>
+      <c r="F67" s="13">
+        <v>98305.0</v>
+      </c>
+      <c r="G67" s="13">
+        <v>983041.0</v>
+      </c>
+      <c r="H67" s="13">
+        <v>1.9922948E7</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="B68" s="16">
+        <v>654.0</v>
+      </c>
+      <c r="C68" s="16">
+        <v>625.0</v>
+      </c>
+      <c r="D68" s="16">
+        <v>741.0</v>
+      </c>
+      <c r="E68" s="16">
+        <v>833.0</v>
+      </c>
+      <c r="F68" s="16">
+        <v>1421.0</v>
+      </c>
+      <c r="G68" s="16">
+        <v>8057.0</v>
+      </c>
+      <c r="H68" s="16">
+        <v>87928.0</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="B69" s="16">
+        <v>770.0</v>
+      </c>
+      <c r="C69" s="16">
+        <v>760.0</v>
+      </c>
+      <c r="D69" s="16">
+        <v>633.0</v>
+      </c>
+      <c r="E69" s="16">
+        <v>770.0</v>
+      </c>
+      <c r="F69" s="16">
+        <v>1095.0</v>
+      </c>
+      <c r="G69" s="16">
+        <v>4809.0</v>
+      </c>
+      <c r="H69" s="16">
+        <v>65735.0</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" s="7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" s="33" t="s">
+        <v>34</v>
+      </c>
+      <c r="B73" s="33" t="s">
+        <v>35</v>
+      </c>
+      <c r="C73" s="33" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" s="34" t="s">
+        <v>37</v>
+      </c>
+      <c r="B74" s="7">
+        <v>769.0</v>
+      </c>
+      <c r="C74" s="7">
+        <v>769.0</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" s="34" t="s">
+        <v>38</v>
+      </c>
+      <c r="B75" s="7">
+        <v>1793.0</v>
+      </c>
+      <c r="C75" s="7">
+        <v>1793.0</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="B76" s="7">
+        <v>4097.0</v>
+      </c>
+      <c r="C76" s="7">
+        <v>4097.0</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="B77" s="7">
+        <v>9217.0</v>
+      </c>
+      <c r="C77" s="7">
+        <v>9217.0</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="18">
+  <mergeCells count="28">
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="A4:C4"/>
+    <mergeCell ref="A6:C6"/>
+    <mergeCell ref="A8:E8"/>
+    <mergeCell ref="I9:M9"/>
+    <mergeCell ref="A9:E9"/>
+    <mergeCell ref="C10:E10"/>
     <mergeCell ref="B11:E11"/>
+    <mergeCell ref="A22:E22"/>
+    <mergeCell ref="C23:E23"/>
+    <mergeCell ref="B24:E24"/>
+    <mergeCell ref="A34:E34"/>
+    <mergeCell ref="A61:G61"/>
+    <mergeCell ref="A63:E63"/>
+    <mergeCell ref="A64:E64"/>
+    <mergeCell ref="F64:H64"/>
+    <mergeCell ref="B65:E65"/>
+    <mergeCell ref="B66:H66"/>
+    <mergeCell ref="A72:G72"/>
     <mergeCell ref="C36:E36"/>
     <mergeCell ref="B37:E37"/>
-    <mergeCell ref="A49:G49"/>
     <mergeCell ref="A51:G51"/>
-    <mergeCell ref="A34:E34"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="A3:C3"/>
-    <mergeCell ref="A8:E8"/>
-    <mergeCell ref="A9:E9"/>
-    <mergeCell ref="I9:M9"/>
-    <mergeCell ref="C23:E23"/>
-    <mergeCell ref="B24:E24"/>
-    <mergeCell ref="C10:E10"/>
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="A6:C6"/>
-    <mergeCell ref="A4:C4"/>
-    <mergeCell ref="A22:E22"/>
+    <mergeCell ref="A52:G52"/>
+    <mergeCell ref="A54:E54"/>
+    <mergeCell ref="B55:E55"/>
+    <mergeCell ref="B56:E56"/>
   </mergeCells>
   <printOptions gridLines="1" horizontalCentered="1"/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.25" right="0.25" top="0.75"/>

</xml_diff>